<commit_message>
Update U3 BOM status
</commit_message>
<xml_diff>
--- a/u3-daughterboard/U3_SMT/U3_BOM.xlsx
+++ b/u3-daughterboard/U3_SMT/U3_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\unified-daughterboard\u3-daughterboard\U3_SMT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3398D2AB-EF39-4CC4-903B-9CF4355FD2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61112E15-7113-44EF-AAC9-C3D73F13E4FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7870" yWindow="5610" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -123,7 +123,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,8 +161,15 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,8 +182,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -234,17 +247,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -270,7 +272,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -299,9 +301,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -310,19 +309,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -614,17 +601,17 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.08984375" style="1" customWidth="1"/>
     <col min="2" max="2" width="39.36328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="58.08984375" style="14" customWidth="1"/>
+    <col min="3" max="3" width="58.08984375" style="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" customWidth="1"/>
     <col min="5" max="5" width="23.1796875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.26953125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="14.26953125" style="10" customWidth="1"/>
     <col min="7" max="7" width="46.26953125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
@@ -636,7 +623,7 @@
       <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="4" t="s">
@@ -645,10 +632,10 @@
       <c r="E1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>12</v>
       </c>
     </row>
@@ -656,120 +643,114 @@
       <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="F2" s="1"/>
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="1">
         <v>2</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
+      <c r="F3" s="1"/>
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
+      <c r="F4" s="1"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
+      <c r="F5" s="1"/>
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
+      <c r="F6" s="1"/>
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="1">
         <v>1</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
+      <c r="F7" s="1"/>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>1</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="10"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>